<commit_message>
feat: generated model outputs, prepared human eval samples, and created evaluation template
</commit_message>
<xml_diff>
--- a/evaluation/human_eval_template.xlsx
+++ b/evaluation/human_eval_template.xlsx
@@ -44,7 +44,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00CCE5FF"/>
-        <bgColor rgb="00CCE5FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -60,11 +59,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,31 +447,26 @@
           <t>Human Evaluation Instructions</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Please rate each code sample on the following criteria:</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Please rate each model-generated comment based on the following criteria:</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1. Correctness (1-5):</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>1. Correctness (1–5):</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -477,7 +474,6 @@
           <t xml:space="preserve">  1 = Completely incorrect/broken</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -485,7 +481,6 @@
           <t xml:space="preserve">  2 = Mostly incorrect with major errors</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -493,7 +488,6 @@
           <t xml:space="preserve">  3 = Partially correct, some issues</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -501,7 +495,6 @@
           <t xml:space="preserve">  4 = Mostly correct, minor issues</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -509,19 +502,16 @@
           <t xml:space="preserve">  5 = Completely correct</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2. Readability (1-5):</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+          <t>2. Readability (1–5):</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -529,7 +519,6 @@
           <t xml:space="preserve">  1 = Unreadable, poorly formatted</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -537,7 +526,6 @@
           <t xml:space="preserve">  2 = Hard to read</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -545,7 +533,6 @@
           <t xml:space="preserve">  3 = Acceptable readability</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -553,27 +540,23 @@
           <t xml:space="preserve">  4 = Good readability</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  5 = Excellent, professional formatting</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
+          <t xml:space="preserve">  5 = Excellent formatting</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3. Usefulness (1-5):</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
+          <t>3. Usefulness (1–5):</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -581,7 +564,6 @@
           <t xml:space="preserve">  1 = Not useful at all</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -589,7 +571,6 @@
           <t xml:space="preserve">  2 = Slightly useful</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -597,7 +578,6 @@
           <t xml:space="preserve">  3 = Moderately useful</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -605,7 +585,6 @@
           <t xml:space="preserve">  4 = Very useful</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -613,11 +592,9 @@
           <t xml:space="preserve">  5 = Production-ready</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -625,15 +602,13 @@
           <t>4. Hallucination Detection:</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Select if the output contains fabricated/incorrect information</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
+          <t xml:space="preserve">  - Mark Yes/No if the model makes up incorrect facts</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -641,7 +616,6 @@
           <t xml:space="preserve">  - Severity: Minor / Moderate / Critical</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -649,7 +623,6 @@
           <t xml:space="preserve">  - Describe the hallucination briefly</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -662,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -674,14 +647,13 @@
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="40" customWidth="1" min="11" max="11"/>
-    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
+    <col width="40" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -692,451 +664,668 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>input</t>
+          <t>code_snippet</t>
         </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>expected</t>
+          <t>generated_comment</t>
         </is>
       </c>
       <c r="D1" s="2" t="inlineStr">
         <is>
-          <t>model_output</t>
+          <t>ground_truth</t>
         </is>
       </c>
       <c r="E1" s="2" t="inlineStr">
         <is>
-          <t>task</t>
+          <t>Correctness (1–5)</t>
         </is>
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Correctness (1-5)</t>
+          <t>Readability (1–5)</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Readability (1-5)</t>
+          <t>Usefulness (1–5)</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Usefulness (1-5)</t>
+          <t>Has Hallucination? (Yes/No)</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Has Hallucination? (Yes/No)</t>
+          <t>Hallucination Severity (Minor/Moderate/Critical)</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>Hallucination Severity (Minor/Moderate/Critical)</t>
+          <t>Hallucination Description</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>Hallucination Description</t>
-        </is>
-      </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="3" t="n">
         <v>83</v>
       </c>
-      <c r="B2" t="n">
-        <v/>
-      </c>
-      <c r="C2" t="n">
-        <v/>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>I'm sorry, but you haven't provided any code for me to generate a docstring for. Could you please provide a Python function or</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>def get(self, df: DataFrame, *mask):
+		"""
+		Return result from the masks request
+		"""</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    df: Input pandas dataframe for operations.
+    mask: Variable length argument to apply different kinds of filters on dataframe
+Returns:
+    DataFrame: Returns a filtered pandas dataframe based on the input masks</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Return result from the masks request</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr"/>
+      <c r="F2" s="3" t="inlineStr"/>
+      <c r="G2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr"/>
+      <c r="I2" s="3" t="inlineStr"/>
+      <c r="J2" s="3" t="inlineStr"/>
+      <c r="K2" s="3" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="3" t="n">
         <v>53</v>
       </c>
-      <c r="B3" t="n">
-        <v/>
-      </c>
-      <c r="C3" t="n">
-        <v/>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>I'm sorry, but you haven't provided any code for a Python documentation generator to analyze. Please provide the specific code that needs to be documented for proper assistance.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>def id(self):
+        """Gets the id of this OperationSortResultsScore.
+        :return: The id of this OperationSortResultsScore.
+        :rtype: str
+        """</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    self: instance of the class
+Returns:
+    The id of this OperationSortResultsScore: string type</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Gets the id of this OperationSortResultsScore.
+        :return: The id of this OperationSortResultsScore.
+        :rtype: str</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="inlineStr"/>
+      <c r="F3" s="3" t="inlineStr"/>
+      <c r="G3" s="3" t="inlineStr"/>
+      <c r="H3" s="3" t="inlineStr"/>
+      <c r="I3" s="3" t="inlineStr"/>
+      <c r="J3" s="3" t="inlineStr"/>
+      <c r="K3" s="3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="B4" t="n">
-        <v/>
-      </c>
-      <c r="C4" t="n">
-        <v/>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>I'm sorry, but your request is incomplete as you didn't provide any code for me to generate a Python docstring for. Could you please provide the specific piece of code you want a documentation comment for?</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>def sample_object_count(self):
+        """
+        Sample the number of objects to place on this particular furniture unit.
+        :return: Number of objects.
+        """</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    self: The instance of the</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>Sample the number of objects to place on this particular furniture unit.
+        :return: Number of objects.</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr"/>
+      <c r="F4" s="3" t="inlineStr"/>
+      <c r="G4" s="3" t="inlineStr"/>
+      <c r="H4" s="3" t="inlineStr"/>
+      <c r="I4" s="3" t="inlineStr"/>
+      <c r="J4" s="3" t="inlineStr"/>
+      <c r="K4" s="3" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="B5" t="n">
-        <v/>
-      </c>
-      <c r="C5" t="n">
-        <v/>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>I'm sorry, but you didn't provide any Python code for me to generate a docstring for. Could you please share more details or the specific Python function/code whose docstring you need? This will help in generating the accurate and clean Python docstring as per your request.</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>def description(self):
+        """Gets the description of this ModifySecurityGroupAttributesRequest.  # noqa: E501
+        :return: The description of this ModifySecurityGroupAttributesRequest.  # noqa: E501
+        :rtype: str
+        """</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    self: Instance of the object itself (used to access</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Gets the description of this ModifySecurityGroupAttributesRequest.  # noqa: E501
+        :return: The description of this ModifySecurityGroupAttributesRequest.  # noqa: E501
+        :rtype: str</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr"/>
+      <c r="F5" s="3" t="inlineStr"/>
+      <c r="G5" s="3" t="inlineStr"/>
+      <c r="H5" s="3" t="inlineStr"/>
+      <c r="I5" s="3" t="inlineStr"/>
+      <c r="J5" s="3" t="inlineStr"/>
+      <c r="K5" s="3" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="B6" t="n">
-        <v/>
-      </c>
-      <c r="C6" t="n">
-        <v/>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>I'm sorry, but your question is incomplete. Could you please provide the code for which you want to generate a Python docstring?</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>def matrix_to_quaternion(matrix, eps=1e-6):
+    """
+    This function is borrowed from https://github.com/kornia/kornia
+    Convert rotation matrix to 4d quaternion vector
+    This algorithm is based on algorithm described in
+    https://github.com/KieranWynn/pyquaternion/blob/master/pyquaternion/quaternion.py#L201
+    :param matrix (N, 3, 3)
+    """</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>a clean Python docstring for the provided code snippet:</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>This function is borrowed from https://github.com/kornia/kornia
+    Convert rotation matrix to 4d quaternion vector
+    This algorithm is based on algorithm described in
+    https://github.com/KieranWynn/pyquaternion/blob/master/pyquaternion/quaternion.py#L201
+    :param matrix (N, 3, 3)</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
+      <c r="I6" s="3" t="inlineStr"/>
+      <c r="J6" s="3" t="inlineStr"/>
+      <c r="K6" s="3" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="B7" t="n">
-        <v/>
-      </c>
-      <c r="C7" t="n">
-        <v/>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>I'm sorry, but I can't provide you with the exact code as your question is incomplete. Could you please provide the Python function for which you need a docstring?</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>def matrix_to_cont_6d(matrix):
+    """
+    :param matrix (*, 3, 3)
+    :returns 6d vector (*, 6)
+    """</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>"Args:\n    matrix (*, 3, 3)\n\nReturns:\n    6d vector (*, 6)"</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>:param matrix (*, 3, 3)
+    :returns 6d vector (*, 6)</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr"/>
+      <c r="F7" s="3" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
+      <c r="I7" s="3" t="inlineStr"/>
+      <c r="J7" s="3" t="inlineStr"/>
+      <c r="K7" s="3" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="B8" t="n">
-        <v/>
-      </c>
-      <c r="C8" t="n">
-        <v/>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>I'm sorry, but you didn't provide any code for me to generate a Python docstring for. Could you please provide the specific code snippet that you want a docstring for? I would be happy to help with that!</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>def disable_replication(self, context, group, volumes):
+        """Disables replication for a group and volumes in the group.
+        :param group: group object
+        :param volumes: list of volume objects in the group
+        :returns: model_update - dict of group updates
+        :returns: volume_model_updates - list of dicts of volume updates
+        """</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    context (object): The context object that contains necessary information for executing the function.
+    group (object): The group object whose replication needs to be disabled.
+    volumes (list): A list of volume objects in the group whose replication needs to be disabled.
+Returns:
+    model_update (dict): A dictionary containing updates related to the group that disables its replication.
+    volume_model_updates (list): A list of dictionaries, each containing updates for a specific volume that disables its replication.</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>Disables replication for a group and volumes in the group.
+        :param group: group object
+        :param volumes: list of volume objects in the group
+        :returns: model_update - dict of group updates
+        :returns: volume_model_updates - list of dicts of volume updates</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr"/>
+      <c r="F8" s="3" t="inlineStr"/>
+      <c r="G8" s="3" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr"/>
+      <c r="I8" s="3" t="inlineStr"/>
+      <c r="J8" s="3" t="inlineStr"/>
+      <c r="K8" s="3" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="3" t="n">
         <v>80</v>
       </c>
-      <c r="B9" t="n">
-        <v/>
-      </c>
-      <c r="C9" t="n">
-        <v/>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>I'm sorry, but you didn't provide any code to generate a docstring for. Could you please provide some code? I'll be glad to help with that!</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>def is_object_in_air(segmask, body_uid):
+    """
+    From the segmask image from a parallel projection, check if the object is balancing over the edge of the workspace.
+    :param segmask: Parallel projection segmask image.
+    :param body_uid: Physics simulation UID of the body.
+    :return: True if object is balancing over workspace, False otherwise.
+    """</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    segmask: Parallel projection segmask image.
+    body_uid: Physics simulation UID of the body.
+Returns:
+    bool: True if object is balancing over workspace, False otherwise.</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>From the segmask image from a parallel projection, check if the object is balancing over the edge of the workspace.
+    :param segmask: Parallel projection segmask image.
+    :param body_uid: Physics simulation UID of the body.
+    :return: True if object is balancing over workspace, False otherwise.</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr"/>
+      <c r="F9" s="3" t="inlineStr"/>
+      <c r="G9" s="3" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr"/>
+      <c r="I9" s="3" t="inlineStr"/>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" s="3" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B10" t="n">
-        <v/>
-      </c>
-      <c r="C10" t="n">
-        <v/>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>I'm sorry, but you haven't provided any code to generate a Python docstring for. Please provide the code that needs a docstring.</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>def get_default_filter_function(self):
+        """Get the default filter_function string.
+        Each driver could overwrite the method to return a well-known
+        default string if it is available.
+        :returns: None
+        """</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    self
+Returns:
+    str: Default filter function as a string</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>Get the default filter_function string.
+        Each driver could overwrite the method to return a well-known
+        default string if it is available.
+        :returns: None</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr"/>
+      <c r="F10" s="3" t="inlineStr"/>
+      <c r="G10" s="3" t="inlineStr"/>
+      <c r="H10" s="3" t="inlineStr"/>
+      <c r="I10" s="3" t="inlineStr"/>
+      <c r="J10" s="3" t="inlineStr"/>
+      <c r="K10" s="3" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="B11" t="n">
-        <v/>
-      </c>
-      <c r="C11" t="n">
-        <v/>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>I'm sorry, but without specific code to generate a Python docstring for, I cannot provide you with an accurate response. Could you please share the code you want me to generate a docstring for?</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>def do_deploy(archive_path):
+    """Distributes an archive to a web server.
+    Args:
+        archive_path (str): The path of the archive to distribute.
+    Returns:
+        If the file doesn't exist at archive_path or an error occurs - False.
+        Otherwise - True.
+    """</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+archive_path (str): The path of the archive to distribute.
+Returns:
+If the file doesn't exist at archive_path or an error occurs - False. Otherwise - True.</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>Distributes an archive to a web server.
+    Args:
+        archive_path (str): The path of the archive to distribute.
+    Returns:
+        If the file doesn't exist at archive_path or an error occurs - False.
+        Otherwise - True.</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr"/>
+      <c r="F11" s="3" t="inlineStr"/>
+      <c r="G11" s="3" t="inlineStr"/>
+      <c r="H11" s="3" t="inlineStr"/>
+      <c r="I11" s="3" t="inlineStr"/>
+      <c r="J11" s="3" t="inlineStr"/>
+      <c r="K11" s="3" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" t="n">
-        <v/>
-      </c>
-      <c r="C12" t="n">
-        <v/>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>I'm sorry, but without knowing what specific code you want a Python docstring for, I can't provide an accurate example. Could you please share the code?</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="A12" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>def transform(self, texts, 
+                    to_lower            = False,
+                    # Remove
+                    rm_email_formatting = False, 
+                    rm_email_header     = False,
+                    rm_email_footer     = False, 
+                    rm_punctuation      = False,
+                    # Placeholders
+                    rp_generic          = False, 
+                    rp_num              = False,
+                    # Tokenize
+                    lemmatize           = False,
+                    rm_stopwords        = False,
+                    return_token        = False,
+                    # Whitespace
+                    remove_whitespace   = True
+                ):
+        """Main run function for cleaning process"""</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+- texts (list of str): A list of text strings to be cleaned
+- to_lower (bool, optional): Whether to convert all characters to lowercase or not. Default is False.
+- rm_email_formatting (bool, optional): Whether to remove email formatting like angle brackets and periods in the middle of words. Default is False.
+- rm_email_header (bool, optional): Whether to remove headers from emails. Default is False.
+- rm_email_footer (bool, optional): Whether to remove footers from emails. Default is False.
+- rm_punctuation (bool, optional): Whether to remove punctuation marks. Default is False.
+- rp_generic (str or bool, optional): If a string, replace all occurrences of this substring with the generic placeholder. If True, use the default placeholder "REDACTED". Default is False.
+- rp_num (bool, optional): Whether to replace numbers with a specific number placeholder. Default is False.
+- lemmatize (bool, optional): Whether to convert words to their base form or not. Default is False.
+- rm_stopwords (bool, optional): Whether to remove common words that usually do not carry much meaningful information. Default is False.
+- return_token (bool, optional): Whether to return the cleaned texts as a list of tokens (words). Default is False.
+- remove_whitespace (bool, optional): Whether to remove all whitespaces including tabs and newlines. Default is True.
+Returns:
+- list of str or str: If `return_token` is set to True, return the cleaned texts as a list of tokens; otherwise, return the cleaned texts as one long string. The cleaning process will be done based on the input arguments provided.</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>Main run function for cleaning process</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr"/>
+      <c r="F12" s="3" t="inlineStr"/>
+      <c r="G12" s="3" t="inlineStr"/>
+      <c r="H12" s="3" t="inlineStr"/>
+      <c r="I12" s="3" t="inlineStr"/>
+      <c r="J12" s="3" t="inlineStr"/>
+      <c r="K12" s="3" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" t="n">
-        <v/>
-      </c>
-      <c r="C13" t="n">
-        <v/>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>I'm sorry, but your request is not clear enough. Could you provide more details about the Python code for which you need a clean docstring? The format of the docstring will depend on what exactly the function does and how it should be used.</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="A13" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>def convert_examples_to_features(examples, label_list, max_seq_length, tokenizer,
+                                 cls_token_at_end=False, cls_token="[CLS]", cls_token_segment_id=1,
+                                 sep_token="[SEP]", pad_on_left=False, pad_token=0, pad_token_segment_id=0,
+                                 sequence_a_segment_id=0, mask_padding_with_zero=True, ):
+    """ Loads a data file into a list of `InputBatch`s
+        `cls_token_at_end` define the location of the CLS token:
+            - False (Default, BERT/XLM pattern): [CLS] + A + [SEP] + B + [SEP]
+            - True (XLNet/GPT pattern): A + [SEP] + B + [SEP] + [CLS]
+        `cls_token_segment_id` define the segment id associated to the CLS token (0 for BERT, 2 for XLNet)
+    """</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    examples: A list of InputExample objects containing the inputs and labels.
+    label_list: The list of all possible labels.
+    max_seq_length: Maximum length of sequences.
+    tokenizer: An instance of a tokenizer that can be used to process text data.
+    cls_token_at_end: A boolean indicating whether the CLS token should be added at the end or not.
+    cls_token: The string representing the CLS token.
+    cls_token_segment_id: The segment id associated with the CLS token.
+    sep_token: The string representing the SEP token.
+    pad_on_left: A boolean indicating whether padding should be added on the left or not.
+    pad_token: The value to use for padding.
+    pad_token_segment_id: The segment id associated with the pad token.
+    sequence_a_segment_id: The segment id for the first sequence in a pair.
+    mask_padding_with_zero: A boolean indicating whether padding tokens should be masked or not.
+Returns:
+    A list of `InputBatch` objects prepared from the input examples, ready to be fed into a model.</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>Loads a data file into a list of `InputBatch`s
+        `cls_token_at_end` define the location of the CLS token:
+            - False (Default, BERT/XLM pattern): [CLS] + A + [SEP] + B + [SEP]
+            - True (XLNet/GPT pattern): A + [SEP] + B + [SEP] + [CLS]
+        `cls_token_segment_id` define the segment id associated to the CLS token (0 for BERT, 2 for XLNet)</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr"/>
+      <c r="F13" s="3" t="inlineStr"/>
+      <c r="G13" s="3" t="inlineStr"/>
+      <c r="H13" s="3" t="inlineStr"/>
+      <c r="I13" s="3" t="inlineStr"/>
+      <c r="J13" s="3" t="inlineStr"/>
+      <c r="K13" s="3" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>3</v>
-      </c>
-      <c r="B14" t="n">
-        <v/>
-      </c>
-      <c r="C14" t="n">
-        <v/>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Based on your instructions, here is a sample Python docstring for a function without any parameters and returning an integer:</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
+      <c r="A14" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>def fit_mods_parallel_processes(X, Y, k_exprs, restarts = 5, optimiser = GPy_optimisers[0], max_retries = 1):
+    '''Concurrently fit models (from a list of kernels) on the same data in as many processes as there are available processor cores using `multiprocessing`'s `Pool`
+    (this function does NOT use GPy's own `parallel` argument, which parallelises within single fits rather than across multiple ones)
+    NOTE: Any code calling this function (however many nested levels in) should be within an "if __name__ == '__main__':" preamble for full OS-agnostic use.
+    '''</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    X (numpy array): Input data matrix
+    Y (numpy array): Output/target values corresponding to input data
+    k_exprs (list of GPy kernels): List of kernel expressions to fit on the data
+    restarts (int, optional): Number of times to restart optimisation. Default is 5
+    optimiser (GPy optimiser instance, optional): Optimiser to use for fitting models. Default is the first element in `GPy_optimisers` list
+    max_retries (int, optional): Maximum number of retries before raising an exception. Default is 1
+Returns:
+    dict: A dictionary containing fitted GPy model instances and their corresponding R2 scores</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>Concurrently fit models (from a list of kernels) on the same data in as many processes as there are available processor cores using `multiprocessing`'s `Pool`
+    (this function does NOT use GPy's own `parallel` argument, which parallelises within single fits rather than across multiple ones)
+    NOTE: Any code calling this function (however many nested levels in) should be within an "if __name__ == '__main__':" preamble for full OS-agnostic use.</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr"/>
+      <c r="F14" s="3" t="inlineStr"/>
+      <c r="G14" s="3" t="inlineStr"/>
+      <c r="H14" s="3" t="inlineStr"/>
+      <c r="I14" s="3" t="inlineStr"/>
+      <c r="J14" s="3" t="inlineStr"/>
+      <c r="K14" s="3" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>4</v>
-      </c>
-      <c r="B15" t="n">
-        <v/>
-      </c>
-      <c r="C15" t="n">
-        <v/>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Based on your requirements, here's a Python docstring for a function that doesn't take any arguments and does not return anything:</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="A15" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>def create_hierarchy_rows(self, new_hierarchy, row_len):
+        """Returns rows list of hierarchy rows that should be put inside
+        data to show new_hierarchy. If hierarchy rows have been added for
+        new_hierarchy already, empty list will be returned. Hierarchy rows
+        will be have not empty: id(if created), type, name and summable fields.
+        Arguments:
+        new_hierarchy -- list representing hierarchy in row in data 
+        row_len -- length of that row, needed create correct hierarchy row
+        """</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Returns rows list of hierarchy rows that should be put inside
+data to show new_hierarchy. If hierarchy rows have been added for
+new_hierarchy already, empty list will be returned. Hierarchy rows
+will be have not empty: id(if created), type, name and summable fields.
+Arguments:
+new_hierarchy -- list representing hierarchy in row in data 
+row_len -- length of that row, needed create correct hierarchy row</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Returns rows list of hierarchy rows that should be put inside
+        data to show new_hierarchy. If hierarchy rows have been added for
+        new_hierarchy already, empty list will be returned. Hierarchy rows
+        will be have not empty: id(if created), type, name and summable fields.
+        Arguments:
+        new_hierarchy -- list representing hierarchy in row in data 
+        row_len -- length of that row, needed create correct hierarchy row</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr"/>
+      <c r="F15" s="3" t="inlineStr"/>
+      <c r="G15" s="3" t="inlineStr"/>
+      <c r="H15" s="3" t="inlineStr"/>
+      <c r="I15" s="3" t="inlineStr"/>
+      <c r="J15" s="3" t="inlineStr"/>
+      <c r="K15" s="3" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>def quaternion_to_matrix(quaternion):
+    """
+    Convert a quaternion to a rotation matrix.
+    Taken from https://github.com/kornia/kornia, based on
+    https://github.com/matthew-brett/transforms3d/blob/8965c48401d9e8e66b6a8c37c65f2fc200a076fa/transforms3d/quaternions.py#L101
+    https://github.com/tensorflow/graphics/blob/master/tensorflow_graphics/geometry/transformation/rotation_matrix_3d.py#L247
+    :param quaternion (N, 4) expects WXYZ order
+    returns rotation matrix (N, 3, 3)
+    """</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Args:
+    quaternion: A N-by-4 tensor in which each row represents a quaternion with elements in WXYZ order.
+Returns:
+    rotation_matrix: A N-by-3-by-3 tensor representing the corresponding rotation matrices. The rotation is performed in XYZ order.</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>Convert a quaternion to a rotation matrix.
+    Taken from https://github.com/kornia/kornia, based on
+    https://github.com/matthew-brett/transforms3d/blob/8965c48401d9e8e66b6a8c37c65f2fc200a076fa/transforms3d/quaternions.py#L101
+    https://github.com/tensorflow/graphics/blob/master/tensorflow_graphics/geometry/transformation/rotation_matrix_3d.py#L247
+    :param quaternion (N, 4) expects WXYZ order
+    returns rotation matrix (N, 3, 3)</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr"/>
+      <c r="F16" s="3" t="inlineStr"/>
+      <c r="G16" s="3" t="inlineStr"/>
+      <c r="H16" s="3" t="inlineStr"/>
+      <c r="I16" s="3" t="inlineStr"/>
+      <c r="J16" s="3" t="inlineStr"/>
+      <c r="K16" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>